<commit_message>
lista excel con formulas
</commit_message>
<xml_diff>
--- a/Datos/Lista1.xlsx
+++ b/Datos/Lista1.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Numero</t>
   </si>
   <si>
-    <t>Fecha de nacimiento</t>
-  </si>
-  <si>
     <t>Genero</t>
   </si>
   <si>
@@ -75,6 +72,27 @@
   </si>
   <si>
     <t>Eva Huarita</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TOTAL M</t>
+  </si>
+  <si>
+    <t>TOTAL  F</t>
   </si>
 </sst>
 </file>
@@ -118,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -135,6 +153,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,199 +440,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="0.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="4">
         <v>37348</v>
       </c>
-      <c r="F2" s="2">
+      <c r="E2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45763</v>
+      </c>
+      <c r="F2" s="10">
+        <f ca="1">INT((E2-D2)/365)</f>
         <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8">
+        <f>IF(G2="Masculino",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>IF(G2="Femenino",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4">
         <v>36982</v>
       </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E11" ca="1" si="0">TODAY()</f>
+        <v>45763</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F11" ca="1" si="1">INT((E3-D3)/365)</f>
         <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H11" si="2">IF(G3="Masculino",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="3">IF(G3="Femenino",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4">
         <v>36519</v>
       </c>
-      <c r="F4" s="2">
-        <v>26</v>
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>36703</v>
       </c>
-      <c r="F5" s="2">
-        <v>25</v>
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4">
         <v>37653</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" ca="1" si="1"/>
         <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4">
         <v>38112</v>
       </c>
-      <c r="F7" s="2">
-        <v>21</v>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>38544</v>
       </c>
-      <c r="F8" s="2">
-        <v>20</v>
+      <c r="E8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="4">
         <v>37502</v>
       </c>
-      <c r="F9" s="2">
-        <v>23</v>
+      <c r="E9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4">
         <v>37014</v>
       </c>
-      <c r="F10" s="2">
-        <v>24</v>
+      <c r="E10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4">
         <v>36659</v>
       </c>
-      <c r="F11" s="2">
-        <v>25</v>
+      <c r="E11" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45763</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="6">
+        <f ca="1">AVERAGE(F2:F11)</f>
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13">
+        <f>SUM(H2:H11)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <f>SUM(I2:I11)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F13:F14)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>